<commit_message>
continued analysis of the problem
Looked at starting positions. Adjusted code to maintain p_state history. analyzed visual probability states for the select_best_p algorythm.
</commit_message>
<xml_diff>
--- a/select best p starting position 41 vs 96.xlsx
+++ b/select best p starting position 41 vs 96.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tm125f\Desktop\github\rabbit-problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF862ABE-6CBE-4BB5-99D0-A51CB42B4C0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F679ED-C2AD-441D-AAD6-802DE38456C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -671,15 +682,25 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
@@ -1955,15 +1976,25 @@
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
@@ -3231,6 +3262,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1109718384"/>
         <c:axId val="1109720880"/>
@@ -4322,7 +4354,7 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A1:D201"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>